<commit_message>
added test cases for bill.zul: canceled but still produced order items (process runs).
</commit_message>
<xml_diff>
--- a/soberano/test_cases/order_collect_test_cases.xlsx
+++ b/soberano/test_cases/order_collect_test_cases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
   <si>
     <t xml:space="preserve">mc3 exchange rate:</t>
   </si>
@@ -128,6 +128,15 @@
   </si>
   <si>
     <t xml:space="preserve">customer5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canceled but still produced items (same for all order’s process runs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not enough rights. A checker can not change an order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order successfully changed</t>
   </si>
 </sst>
 </file>
@@ -139,7 +148,7 @@
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -168,6 +177,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -217,7 +231,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -252,6 +266,26 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -275,10 +309,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ74"/>
+  <dimension ref="A1:AMJ76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H27" activeCellId="0" sqref="H27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1106,27 +1140,147 @@
       <c r="AMI27" s="7"/>
       <c r="AMJ27" s="7"/>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E35" s="0"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E36" s="0"/>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E71" s="9"/>
-      <c r="F71" s="9"/>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E72" s="9"/>
-      <c r="F72" s="9"/>
+    <row r="28" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="10"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="AMF28" s="10"/>
+      <c r="AMG28" s="10"/>
+      <c r="AMH28" s="10"/>
+      <c r="AMI28" s="10"/>
+      <c r="AMJ28" s="10"/>
+    </row>
+    <row r="29" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="AMF29" s="7"/>
+      <c r="AMG29" s="7"/>
+      <c r="AMH29" s="7"/>
+      <c r="AMI29" s="7"/>
+      <c r="AMJ29" s="7"/>
+    </row>
+    <row r="30" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="7" t="n">
+        <v>1004</v>
+      </c>
+      <c r="F30" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="AMF30" s="7"/>
+      <c r="AMG30" s="7"/>
+      <c r="AMH30" s="7"/>
+      <c r="AMI30" s="7"/>
+      <c r="AMJ30" s="7"/>
+    </row>
+    <row r="31" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="5" t="n">
+        <v>1004</v>
+      </c>
+      <c r="F31" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="AMF31" s="7"/>
+      <c r="AMG31" s="7"/>
+      <c r="AMH31" s="7"/>
+      <c r="AMI31" s="7"/>
+      <c r="AMJ31" s="7"/>
+    </row>
+    <row r="32" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="5" t="n">
+        <v>1005</v>
+      </c>
+      <c r="F32" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="AMF32" s="7"/>
+      <c r="AMG32" s="7"/>
+      <c r="AMH32" s="7"/>
+      <c r="AMI32" s="7"/>
+      <c r="AMJ32" s="7"/>
+    </row>
+    <row r="33" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="5" t="n">
+        <v>1008</v>
+      </c>
+      <c r="F33" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="AMF33" s="7"/>
+      <c r="AMG33" s="7"/>
+      <c r="AMH33" s="7"/>
+      <c r="AMI33" s="7"/>
+      <c r="AMJ33" s="7"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="0"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="0"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E74" s="0"/>
-      <c r="F74" s="0"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E76" s="0"/>
+      <c r="F76" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
buggy. after order reopening, stock isn't the expected.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/order_collect_test_cases.xlsx
+++ b/soberano/test_cases/order_collect_test_cases.xlsx
@@ -148,7 +148,7 @@
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -177,13 +177,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +189,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -231,7 +232,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -264,27 +265,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -301,6 +298,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF81D41A"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -311,8 +368,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="30:33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -502,56 +559,56 @@
       <c r="AMI6" s="7"/>
       <c r="AMJ6" s="7"/>
     </row>
-    <row r="7" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
+    <row r="7" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="5" t="n">
+      <c r="C7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="8" t="n">
         <v>1002</v>
       </c>
-      <c r="F7" s="5" t="n">
+      <c r="F7" s="8" t="n">
         <v>10.32067802</v>
       </c>
-      <c r="G7" s="5" t="n">
+      <c r="G7" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="H7" s="5" t="n">
+      <c r="H7" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="5" t="n">
+      <c r="I7" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="J7" s="5" t="n">
+      <c r="J7" s="8" t="n">
         <f aca="false">G7*E2+1+I7*E3-F7</f>
         <v>-1.23442475970694</v>
       </c>
-      <c r="K7" s="5" t="n">
+      <c r="K7" s="8" t="n">
         <f aca="false">G7*E2+H7+I7*E3</f>
         <v>9.08625326029306</v>
       </c>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="AMF7" s="7"/>
-      <c r="AMG7" s="7"/>
-      <c r="AMH7" s="7"/>
-      <c r="AMI7" s="7"/>
-      <c r="AMJ7" s="7"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="AMF7" s="10"/>
+      <c r="AMG7" s="10"/>
+      <c r="AMH7" s="10"/>
+      <c r="AMI7" s="10"/>
+      <c r="AMJ7" s="10"/>
     </row>
     <row r="8" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="7"/>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="11" t="s">
         <v>21</v>
       </c>
       <c r="O8" s="6"/>
@@ -562,36 +619,36 @@
       <c r="AMI8" s="7"/>
       <c r="AMJ8" s="7"/>
     </row>
-    <row r="9" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
+    <row r="9" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="5" t="n">
+      <c r="C9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="8" t="n">
         <f aca="false">10000.901+6</f>
         <v>10006.901</v>
       </c>
-      <c r="G9" s="5" t="n">
+      <c r="G9" s="8" t="n">
         <f aca="false">23456.09876+1-J6</f>
         <v>23453.0810032582</v>
       </c>
-      <c r="H9" s="5" t="n">
+      <c r="H9" s="8" t="n">
         <f aca="false">54321.2345+7</f>
         <v>54328.2345</v>
       </c>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="AMF9" s="7"/>
-      <c r="AMG9" s="7"/>
-      <c r="AMH9" s="7"/>
-      <c r="AMI9" s="7"/>
-      <c r="AMJ9" s="7"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="AMF9" s="10"/>
+      <c r="AMG9" s="10"/>
+      <c r="AMH9" s="10"/>
+      <c r="AMI9" s="10"/>
+      <c r="AMJ9" s="10"/>
     </row>
     <row r="10" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
@@ -742,13 +799,13 @@
     </row>
     <row r="14" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="7"/>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="11" t="s">
         <v>21</v>
       </c>
       <c r="O14" s="6"/>
@@ -882,13 +939,13 @@
     </row>
     <row r="19" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E19" s="7"/>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="11" t="s">
         <v>21</v>
       </c>
       <c r="O19" s="6"/>
@@ -999,13 +1056,13 @@
     </row>
     <row r="23" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="7"/>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="H23" s="11" t="s">
         <v>21</v>
       </c>
       <c r="O23" s="6"/>
@@ -1092,13 +1149,13 @@
     </row>
     <row r="26" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E26" s="7"/>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H26" s="8" t="s">
+      <c r="H26" s="11" t="s">
         <v>21</v>
       </c>
       <c r="O26" s="6"/>
@@ -1140,15 +1197,8 @@
       <c r="AMI27" s="7"/>
       <c r="AMJ27" s="7"/>
     </row>
-    <row r="28" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E28" s="10"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="AMF28" s="10"/>
-      <c r="AMG28" s="10"/>
-      <c r="AMH28" s="10"/>
-      <c r="AMI28" s="10"/>
-      <c r="AMJ28" s="10"/>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="0"/>
     </row>
     <row r="29" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D29" s="7"/>
@@ -1168,7 +1218,7 @@
       <c r="A30" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C30" s="5" t="s">
@@ -1267,12 +1317,12 @@
       <c r="E38" s="0"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E75" s="3"/>

</xml_diff>